<commit_message>
added awc end to end
</commit_message>
<xml_diff>
--- a/RESTAPIFlight/DataQueries/Flights_REST1/~$SampleAppData.xlsx
+++ b/RESTAPIFlight/DataQueries/Flights_REST1/~$SampleAppData.xlsx
@@ -274,17 +274,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -589,7 +589,7 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -600,7 +600,7 @@
     <col min="7" max="7" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.078125" style="2"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -616,7 +616,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -628,7 +628,7 @@
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -645,7 +645,7 @@
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>78680</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -654,7 +654,7 @@
       <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="6">
         <v>196.40000000000001</v>
       </c>
     </row>
@@ -671,7 +671,7 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>78587</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -680,7 +680,7 @@
       <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="6">
         <v>166.19999999999999</v>
       </c>
     </row>
@@ -697,7 +697,7 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>78678</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -706,7 +706,7 @@
       <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="6">
         <v>104</v>
       </c>
     </row>
@@ -723,7 +723,7 @@
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>78677</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -732,7 +732,7 @@
       <c r="G5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="6">
         <v>253.59999999999999</v>
       </c>
     </row>
@@ -749,7 +749,7 @@
       <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>78801</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -758,7 +758,7 @@
       <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="6">
         <v>173.47</v>
       </c>
     </row>
@@ -775,7 +775,7 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>78676</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -784,7 +784,7 @@
       <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="6">
         <v>163.69999999999999</v>
       </c>
     </row>
@@ -801,7 +801,7 @@
       <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>78674</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -810,7 +810,7 @@
       <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="6">
         <v>112.2</v>
       </c>
     </row>
@@ -827,7 +827,7 @@
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>78676</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -836,7 +836,7 @@
       <c r="G9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="6">
         <v>121.47</v>
       </c>
     </row>

</xml_diff>